<commit_message>
BOM 2 button version small fixes
</commit_message>
<xml_diff>
--- a/CFO_BODYSEQ/documentation/CFO BODYSEQ 2 button version/BOM.xlsx
+++ b/CFO_BODYSEQ/documentation/CFO BODYSEQ 2 button version/BOM.xlsx
@@ -126,9 +126,6 @@
     <t>LED resistors</t>
   </si>
   <si>
-    <t>bodyswitch pulldown resistors</t>
-  </si>
-  <si>
     <t>color code: brown, black, red</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>thumbwheel pot</t>
   </si>
   <si>
-    <t>CFO BODYSEQ BILL OF MATERIALS</t>
-  </si>
-  <si>
     <t>IC socket</t>
   </si>
   <si>
@@ -165,10 +159,16 @@
     <t>R11, R12, R13, R14, R15, R16, R17, R18, R19, R20</t>
   </si>
   <si>
-    <t>S1, S2, S3</t>
-  </si>
-  <si>
-    <t>D1, D2, D3, D4, D5, D6, D8, D9, D10</t>
+    <t>S1, S2,</t>
+  </si>
+  <si>
+    <t>CFO BODYSEQ 2 BUTTON VERSION BILL OF MATERIALS</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10</t>
+  </si>
+  <si>
+    <t>bodyswitch pulldown + op amp resistors</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -651,7 +651,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24">
@@ -712,13 +712,13 @@
     </row>
     <row r="6" spans="1:4" ht="36">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>27</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="9" spans="1:4" ht="24">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4">
@@ -763,7 +763,7 @@
     </row>
     <row r="10" spans="1:4" ht="24">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4">
@@ -772,7 +772,7 @@
     </row>
     <row r="11" spans="1:4" ht="36">
       <c r="A11" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4">
@@ -781,7 +781,7 @@
     </row>
     <row r="12" spans="1:4" ht="36">
       <c r="A12" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="4">
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="36">
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="36">
@@ -845,10 +845,10 @@
         <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>34</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="18" spans="1:7" ht="48">
       <c r="A18" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>18</v>
@@ -865,7 +865,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G18" s="6"/>
     </row>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="48">
@@ -894,22 +894,22 @@
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="24">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7">

</xml_diff>